<commit_message>
[Add] Fine tuning transfer learning
</commit_message>
<xml_diff>
--- a/images/metrics.xlsx
+++ b/images/metrics.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9346ADC5-9884-45E8-A6BF-552B59F46563}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5228CA-3BEC-4984-AE6C-91ED87090B9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1800" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5400" yWindow="3045" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>techniques</t>
   </si>
@@ -43,22 +43,25 @@
     <t>TFKeras_optimized</t>
   </si>
   <si>
-    <t>TFKeras_optimized+TL</t>
-  </si>
-  <si>
     <t>pytorch_optimized</t>
   </si>
   <si>
-    <t>pytorch_optimized+TL</t>
-  </si>
-  <si>
     <t>pytorch_optimized+DLv2</t>
   </si>
   <si>
     <t>FastAI</t>
   </si>
   <si>
-    <t>pytorch_optimized+TL+DLv2</t>
+    <t>pytorch+TL</t>
+  </si>
+  <si>
+    <t>pytorch+TL+DLv2</t>
+  </si>
+  <si>
+    <t>py_torch+TL_Optimized+DLv2</t>
+  </si>
+  <si>
+    <t>TFKeras+TL</t>
   </si>
 </sst>
 </file>
@@ -376,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +450,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>0.7</v>
@@ -461,7 +464,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>0.95</v>
@@ -475,7 +478,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>0.63</v>
@@ -489,7 +492,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0.79</v>
@@ -503,7 +506,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>0.76</v>
@@ -517,7 +520,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0.95</v>
@@ -531,7 +534,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>0.52</v>
@@ -545,7 +548,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <v>0.8</v>
@@ -559,7 +562,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>0.72</v>
@@ -573,7 +576,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -587,7 +590,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>0.74</v>
@@ -601,20 +604,34 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>0.95</v>
       </c>
       <c r="C16">
-        <v>1.34</v>
+        <v>134</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>0.82</v>
+      </c>
+      <c r="C17">
+        <v>343</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D16" xr:uid="{F46C74CB-B9A0-41B4-B94C-63F9BFD6838E}"/>
+  <autoFilter ref="A1:D17" xr:uid="{F46C74CB-B9A0-41B4-B94C-63F9BFD6838E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>